<commit_message>
Fixed issues in the HL7, now works
</commit_message>
<xml_diff>
--- a/CRVS Spec from Pharmacy.xlsx
+++ b/CRVS Spec from Pharmacy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N. Bunker\Dropbox (AIRA)\Shared AIRA Files\COVID-19 Pandemic Response\Puente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\immregistries\Puente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0D7A0B-79C4-4231-8199-094022295B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B15D8DF-2A76-4B3A-81B4-72C0604B0433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{345F94AC-3EB1-4843-98B7-0CF9FCF4D743}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{345F94AC-3EB1-4843-98B7-0CF9FCF4D743}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary Background" sheetId="28" state="hidden" r:id="rId1"/>
@@ -3702,6 +3702,15 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3734,15 +3743,6 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6235,122 +6235,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="137" t="s">
+      <c r="A1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="137"/>
-      <c r="K1" s="137"/>
+      <c r="B1" s="140"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="140"/>
+      <c r="K1" s="140"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="137"/>
-      <c r="B2" s="137"/>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
+      <c r="A2" s="140"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
+      <c r="H2" s="140"/>
+      <c r="I2" s="140"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
     </row>
     <row r="3" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
     </row>
     <row r="4" spans="1:11" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="139"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="139"/>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
+      <c r="B4" s="142"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="142"/>
+      <c r="F4" s="142"/>
+      <c r="G4" s="142"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="142"/>
     </row>
     <row r="5" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="140" t="s">
+      <c r="A5" s="143" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="140"/>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="140"/>
-      <c r="H5" s="140"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
     </row>
     <row r="6" spans="1:11" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="141" t="s">
+      <c r="A6" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="141"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="141"/>
-      <c r="G6" s="141"/>
-      <c r="H6" s="141"/>
-      <c r="I6" s="141"/>
-      <c r="J6" s="141"/>
-      <c r="K6" s="141"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144"/>
+      <c r="E6" s="144"/>
+      <c r="F6" s="144"/>
+      <c r="G6" s="144"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="144"/>
+      <c r="J6" s="144"/>
+      <c r="K6" s="144"/>
     </row>
     <row r="7" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="142" t="s">
+      <c r="A7" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="142"/>
-      <c r="C7" s="142"/>
-      <c r="D7" s="142"/>
-      <c r="E7" s="142"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="142"/>
-      <c r="I7" s="142"/>
-      <c r="J7" s="142"/>
-      <c r="K7" s="142"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
+      <c r="F7" s="145"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="145"/>
     </row>
     <row r="8" spans="1:11" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="136" t="s">
+      <c r="A8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="136"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
+      <c r="B8" s="139"/>
+      <c r="C8" s="139"/>
+      <c r="D8" s="139"/>
+      <c r="E8" s="139"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="139"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0"/>
@@ -7547,21 +7547,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="104" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="146" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="144"/>
-      <c r="C1" s="144"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="143" t="s">
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="146" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="145"/>
-      <c r="G1" s="144" t="s">
+      <c r="F1" s="148"/>
+      <c r="G1" s="147" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="144"/>
-      <c r="I1" s="145"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="148"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -42409,10 +42409,10 @@
   <dimension ref="A1:J451"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42427,21 +42427,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="104" customFormat="1" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="149" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146" t="s">
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149" t="s">
         <v>359</v>
       </c>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146" t="s">
+      <c r="F1" s="149"/>
+      <c r="G1" s="149" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="149"/>
       <c r="J1" s="95"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -42504,7 +42504,7 @@
       <c r="I3" s="102">
         <v>568971356</v>
       </c>
-      <c r="J3" s="147" t="s">
+      <c r="J3" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42536,7 +42536,7 @@
       <c r="I4" s="101" t="s">
         <v>184</v>
       </c>
-      <c r="J4" s="148" t="s">
+      <c r="J4" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -42566,7 +42566,7 @@
         <v>177</v>
       </c>
       <c r="I5" s="101"/>
-      <c r="J5" s="148" t="s">
+      <c r="J5" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -42598,7 +42598,7 @@
       <c r="I6" s="101">
         <v>135498413</v>
       </c>
-      <c r="J6" s="149" t="s">
+      <c r="J6" s="138" t="s">
         <v>175</v>
       </c>
     </row>
@@ -42630,7 +42630,7 @@
       <c r="I7" s="101" t="s">
         <v>753</v>
       </c>
-      <c r="J7" s="149" t="s">
+      <c r="J7" s="138" t="s">
         <v>175</v>
       </c>
     </row>
@@ -42662,7 +42662,7 @@
       <c r="I8" s="101" t="s">
         <v>754</v>
       </c>
-      <c r="J8" s="147" t="s">
+      <c r="J8" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42694,7 +42694,7 @@
       <c r="I9" s="101" t="s">
         <v>755</v>
       </c>
-      <c r="J9" s="149" t="s">
+      <c r="J9" s="138" t="s">
         <v>175</v>
       </c>
     </row>
@@ -42726,7 +42726,7 @@
       <c r="I10" s="123">
         <v>24985</v>
       </c>
-      <c r="J10" s="149" t="s">
+      <c r="J10" s="138" t="s">
         <v>175</v>
       </c>
     </row>
@@ -42758,7 +42758,7 @@
       <c r="I11" s="102" t="s">
         <v>211</v>
       </c>
-      <c r="J11" s="147" t="s">
+      <c r="J11" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42790,7 +42790,7 @@
       <c r="I12" s="102" t="s">
         <v>756</v>
       </c>
-      <c r="J12" s="147" t="s">
+      <c r="J12" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42822,7 +42822,7 @@
       <c r="I13" s="102" t="s">
         <v>757</v>
       </c>
-      <c r="J13" s="147" t="s">
+      <c r="J13" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42854,7 +42854,7 @@
       <c r="I14" s="102" t="s">
         <v>758</v>
       </c>
-      <c r="J14" s="147" t="s">
+      <c r="J14" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42886,7 +42886,7 @@
       <c r="I15" s="102">
         <v>13121</v>
       </c>
-      <c r="J15" s="147" t="s">
+      <c r="J15" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42918,7 +42918,7 @@
       <c r="I16" s="102" t="s">
         <v>230</v>
       </c>
-      <c r="J16" s="147" t="s">
+      <c r="J16" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42950,7 +42950,7 @@
       <c r="I17" s="102">
         <v>30301</v>
       </c>
-      <c r="J17" s="147" t="s">
+      <c r="J17" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -42982,7 +42982,7 @@
       <c r="I18" s="101" t="s">
         <v>238</v>
       </c>
-      <c r="J18" s="147" t="s">
+      <c r="J18" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43014,7 +43014,7 @@
       <c r="I19" s="101" t="s">
         <v>243</v>
       </c>
-      <c r="J19" s="147" t="s">
+      <c r="J19" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43046,7 +43046,7 @@
       <c r="I20" s="101" t="s">
         <v>246</v>
       </c>
-      <c r="J20" s="147" t="s">
+      <c r="J20" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43078,7 +43078,7 @@
       <c r="I21" s="101" t="s">
         <v>249</v>
       </c>
-      <c r="J21" s="147" t="s">
+      <c r="J21" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43110,7 +43110,7 @@
       <c r="I22" s="101" t="s">
         <v>252</v>
       </c>
-      <c r="J22" s="147" t="s">
+      <c r="J22" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43142,7 +43142,7 @@
       <c r="I23" s="101" t="s">
         <v>255</v>
       </c>
-      <c r="J23" s="147" t="s">
+      <c r="J23" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43174,7 +43174,7 @@
       <c r="I24" s="101" t="s">
         <v>260</v>
       </c>
-      <c r="J24" s="147" t="s">
+      <c r="J24" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43206,7 +43206,7 @@
       <c r="I25" s="123">
         <v>44180</v>
       </c>
-      <c r="J25" s="149" t="s">
+      <c r="J25" s="138" t="s">
         <v>175</v>
       </c>
     </row>
@@ -43238,7 +43238,7 @@
       <c r="I26" s="125" t="s">
         <v>269</v>
       </c>
-      <c r="J26" s="149" t="s">
+      <c r="J26" s="138" t="s">
         <v>175</v>
       </c>
     </row>
@@ -43268,7 +43268,7 @@
         <v>183</v>
       </c>
       <c r="I27" s="125"/>
-      <c r="J27" s="147" t="s">
+      <c r="J27" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43300,7 +43300,7 @@
       <c r="I28" s="101" t="s">
         <v>279</v>
       </c>
-      <c r="J28" s="147" t="s">
+      <c r="J28" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43332,7 +43332,7 @@
       <c r="I29" s="102" t="s">
         <v>283</v>
       </c>
-      <c r="J29" s="147" t="s">
+      <c r="J29" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43364,7 +43364,7 @@
       <c r="I30" s="123">
         <v>44365</v>
       </c>
-      <c r="J30" s="147" t="s">
+      <c r="J30" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43396,7 +43396,7 @@
       <c r="I31" s="102" t="s">
         <v>291</v>
       </c>
-      <c r="J31" s="147" t="s">
+      <c r="J31" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43428,7 +43428,7 @@
       <c r="I32" s="102" t="s">
         <v>296</v>
       </c>
-      <c r="J32" s="147" t="s">
+      <c r="J32" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43460,7 +43460,7 @@
       <c r="I33" s="101">
         <v>2</v>
       </c>
-      <c r="J33" s="148" t="s">
+      <c r="J33" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43492,7 +43492,7 @@
       <c r="I34" s="102" t="s">
         <v>305</v>
       </c>
-      <c r="J34" s="148" t="s">
+      <c r="J34" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43524,7 +43524,7 @@
       <c r="I35" s="102" t="s">
         <v>309</v>
       </c>
-      <c r="J35" s="147" t="s">
+      <c r="J35" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43556,7 +43556,7 @@
       <c r="I36" s="101" t="s">
         <v>313</v>
       </c>
-      <c r="J36" s="147" t="s">
+      <c r="J36" s="136" t="s">
         <v>761</v>
       </c>
     </row>
@@ -43588,7 +43588,7 @@
       <c r="I37" s="101">
         <v>123456</v>
       </c>
-      <c r="J37" s="148" t="s">
+      <c r="J37" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43620,7 +43620,7 @@
       <c r="I38" s="101">
         <v>17</v>
       </c>
-      <c r="J38" s="148" t="s">
+      <c r="J38" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43652,7 +43652,7 @@
       <c r="I39" s="101" t="s">
         <v>325</v>
       </c>
-      <c r="J39" s="148" t="s">
+      <c r="J39" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43684,7 +43684,7 @@
       <c r="I40" s="101" t="s">
         <v>329</v>
       </c>
-      <c r="J40" s="148" t="s">
+      <c r="J40" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43716,7 +43716,7 @@
       <c r="I41" s="101" t="s">
         <v>333</v>
       </c>
-      <c r="J41" s="148" t="s">
+      <c r="J41" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43748,7 +43748,7 @@
       <c r="I42" s="102">
         <v>13121</v>
       </c>
-      <c r="J42" s="148" t="s">
+      <c r="J42" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43780,7 +43780,7 @@
       <c r="I43" s="102" t="s">
         <v>230</v>
       </c>
-      <c r="J43" s="148" t="s">
+      <c r="J43" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43812,7 +43812,7 @@
       <c r="I44" s="101">
         <v>30301</v>
       </c>
-      <c r="J44" s="148" t="s">
+      <c r="J44" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43844,8 +43844,8 @@
       <c r="I45" s="101" t="s">
         <v>351</v>
       </c>
-      <c r="J45" s="148" t="s">
-        <v>762</v>
+      <c r="J45" s="138" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="104" customFormat="1" ht="299.25" x14ac:dyDescent="0.25">
@@ -43876,7 +43876,7 @@
       <c r="I46" s="97" t="s">
         <v>305</v>
       </c>
-      <c r="J46" s="148" t="s">
+      <c r="J46" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -43908,7 +43908,7 @@
       <c r="I47" s="97" t="s">
         <v>358</v>
       </c>
-      <c r="J47" s="148" t="s">
+      <c r="J47" s="137" t="s">
         <v>762</v>
       </c>
     </row>
@@ -51643,19 +51643,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="cfea98c8-b831-451c-9715-a60f69f25121">
-      <UserInfo>
-        <DisplayName>Fath, Janet (CDC/DDID/NCIRD/ISD)</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51879,28 +51872,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="cfea98c8-b831-451c-9715-a60f69f25121">
+      <UserInfo>
+        <DisplayName>Fath, Janet (CDC/DDID/NCIRD/ISD)</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB03E680-7482-436B-AF75-43667D9850A9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55C6105D-81FB-48B6-BC11-6EBDD123A930}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="af68c486-4bca-4ffa-9149-95e4479ab26f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cfea98c8-b831-451c-9715-a60f69f25121"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -51926,9 +51916,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55C6105D-81FB-48B6-BC11-6EBDD123A930}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB03E680-7482-436B-AF75-43667D9850A9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="af68c486-4bca-4ffa-9149-95e4479ab26f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cfea98c8-b831-451c-9715-a60f69f25121"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>